<commit_message>
chore: even more finishing touches
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -397,13 +397,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>assignee</v>
+      </c>
+      <c r="B1" t="str">
+        <v>reward</v>
+      </c>
+      <c r="C1" t="str">
+        <v>permit1</v>
+      </c>
+      <c r="D1" t="str">
+        <v>permit2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>devpanther</v>
+      </c>
+      <c r="B2">
+        <v>159.15</v>
+      </c>
+      <c r="C2" t="str">
+        <v>https://pay.ubq.fi?claim=eyJwZXJtaXQiOnsicGVybWl0dGVkIjp7InRva2VuIjoiMHhlOTFEMTUzRTBiNDE1MThBMkNlOERkM0Q3OTQ0RmE4NjM0NjNhOTdkIiwiYW1vdW50IjoiMTUwMDAwMDAwMDAwMDAwMDAwMDAwIn0sIm5vbmNlIjoiNTk5NDM2NjEwMjQxMzM0NDI5MjYzNjE2ODYxMTA5MDc4NjEwNTk2MzQxOTQxMzYzMzQ0MzM0OTU0NTY1NjYxMjQwNjMwNTc4NDg1OTUiLCJkZWFkbGluZSI6IjExNTc5MjA4OTIzNzMxNjE5NTQyMzU3MDk4NTAwODY4NzkwNzg1MzI2OTk4NDY2NTY0MDU2NDAzOTQ1NzU4NDAwNzkxMzEyOTYzOTkzNSJ9LCJ0cmFuc2ZlckRldGFpbHMiOnsidG8iOiIweGY3NkYxQUNCNjYwMjBmODkzYzk1MzcxZjc0MDU0OUYzMTJERUEzZjEiLCJyZXF1ZXN0ZWRBbW91bnQiOiIxNTAwMDAwMDAwMDAwMDAwMDAwMDAifSwib3duZXIiOiIweGY4N2NhNDU4M0M3OTIyMTJlNTI3MjBkMTI3RTdFMEEzOEI4MThhRDEiLCJzaWduYXR1cmUiOiIweDBiMjQyNDg2N2FmOGU0YTM0NGExZjU4YWMwZTkxMjY3MDFhODliZjBmY2RiOTVlMTlmNzUxZmViOWVlODVmNzQ2MzY0ZjE0NzMzNTdmMGQ3ZDExNjkxZjVlN2NjNzM4MTM3NzJjYTJkNzNhZTcxZjk2NWRlZTY2YTgwZGJhZDI2MWIifQ==&amp;network=100</v>
+      </c>
+      <c r="D2" t="str">
+        <v>https://pay.ubq.fi?claim=eyJwZXJtaXQiOnsicGVybWl0dGVkIjp7InRva2VuIjoiMHhlOTFEMTUzRTBiNDE1MThBMkNlOERkM0Q3OTQ0RmE4NjM0NjNhOTdkIiwiYW1vdW50IjoiOTE1MDAwMDAwMDAwMDAwMDAwMCJ9LCJub25jZSI6IjQ1MDg0OTkyMjcxODgwMjM1MDg5NDg0MTE3ODE3MDk4MDk2MzU5MDIzOTI0MTQ1NTA2MDM0OTk3MzM3MDQ0NzIyNTExMzM2NTU2NjY4IiwiZGVhZGxpbmUiOiIxMTU3OTIwODkyMzczMTYxOTU0MjM1NzA5ODUwMDg2ODc5MDc4NTMyNjk5ODQ2NjU2NDA1NjQwMzk0NTc1ODQwMDc5MTMxMjk2Mzk5MzUifSwidHJhbnNmZXJEZXRhaWxzIjp7InRvIjoiMHhmNzZGMUFDQjY2MDIwZjg5M2M5NTM3MWY3NDA1NDlGMzEyREVBM2YxIiwicmVxdWVzdGVkQW1vdW50IjoiOTE1MDAwMDAwMDAwMDAwMDAwMCJ9LCJvd25lciI6IjB4Zjg3Y2E0NTgzQzc5MjIxMmU1MjcyMGQxMjdFN0UwQTM4QjgxOGFEMSIsInNpZ25hdHVyZSI6IjB4YzRjOWEzMWM4OTFjODZmNzRhOTExNzBhZDBkYzQ3YjNjMGU3OTQxNTIwYTQ0MDBjMTg4Zjc4YmJjMzM3NzIwZjAxZDM3OTE1ZDZjNDFkOTdkNzFhYjVmYjZmZjNlZTU4MTlmYjk1YWNjYzA5OWMyNTViNTBiNDBlM2FkNjJiNDQxYyJ9&amp;network=100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>pavlovcik</v>
+      </c>
+      <c r="B3">
+        <v>27.3</v>
+      </c>
+      <c r="C3" t="str">
+        <v>https://pay.ubq.fi?claim=eyJwZXJtaXQiOnsicGVybWl0dGVkIjp7InRva2VuIjoiMHhlOTFEMTUzRTBiNDE1MThBMkNlOERkM0Q3OTQ0RmE4NjM0NjNhOTdkIiwiYW1vdW50IjoiMjczMDAwMDAwMDAwMDAwMDAwMDAifSwibm9uY2UiOiIyNjAwNzgzNzczNTE2ODg2MTUxMTA3ODM3MjA1OTcyNjc4OTEzODgxMDExMDM4ODc3NzU0NzAwOTUxMzYxMTkwNjg1ODIyODYwMDU1MiIsImRlYWRsaW5lIjoiMTE1NzkyMDg5MjM3MzE2MTk1NDIzNTcwOTg1MDA4Njg3OTA3ODUzMjY5OTg0NjY1NjQwNTY0MDM5NDU3NTg0MDA3OTEzMTI5NjM5OTM1In0sInRyYW5zZmVyRGV0YWlscyI6eyJ0byI6IjB4NDAwN0NFMjA4M2M3RjNFMTgwOTdhZUIzQTM5YmI4ZUMxNDlhMzQxZCIsInJlcXVlc3RlZEFtb3VudCI6IjI3MzAwMDAwMDAwMDAwMDAwMDAwIn0sIm93bmVyIjoiMHhmODdjYTQ1ODNDNzkyMjEyZTUyNzIwZDEyN0U3RTBBMzhCODE4YUQxIiwic2lnbmF0dXJlIjoiMHhjNmJmMGQyYmY1YjU1MTYwODFkYjE4NzgxNmFlODFiN2E3MjgzYmQ5YzdhMjhiNDZlZDUzNzQxN2FlMmUzMGEzMTUzODNhYWFmNTQ0NmZiODYxOGVlZjQxMmRhNGFmM2ViNDAyYzMwNTU1MGRhMTNlOGY4YmE5MGFkZjc0MTE1OTFjIn0=&amp;network=100</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>